<commit_message>
[ADD] update reports for the latest database
</commit_message>
<xml_diff>
--- a/src/protrend/report/integration_report.xlsx
+++ b/src/protrend/report/integration_report.xlsx
@@ -253,10 +253,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -634,7 +634,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -681,7 +681,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
@@ -726,7 +726,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
@@ -771,7 +771,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
@@ -816,7 +816,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -863,7 +863,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
@@ -908,7 +908,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
@@ -953,7 +953,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
@@ -998,7 +998,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1045,7 +1045,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1090,7 +1090,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1135,7 +1135,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1180,7 +1180,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1227,7 +1227,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1272,7 +1272,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1317,7 +1317,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1362,7 +1362,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1409,7 +1409,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1454,7 +1454,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1499,7 +1499,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1544,7 +1544,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1591,7 +1591,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="1" t="s">
         <v>17</v>
       </c>
@@ -1636,7 +1636,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="1" t="s">
         <v>18</v>
       </c>
@@ -1681,7 +1681,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1728,7 +1728,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="1" t="s">
         <v>16</v>
       </c>
@@ -1773,7 +1773,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
@@ -1818,7 +1818,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="1" t="s">
         <v>18</v>
       </c>
@@ -1863,7 +1863,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1910,7 +1910,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="1" t="s">
         <v>16</v>
       </c>
@@ -1955,7 +1955,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="1" t="s">
         <v>17</v>
       </c>
@@ -2000,7 +2000,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="1" t="s">
         <v>18</v>
       </c>
@@ -2045,7 +2045,7 @@
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2092,7 +2092,7 @@
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A34" s="8"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="1" t="s">
         <v>16</v>
       </c>
@@ -2137,7 +2137,7 @@
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="1" t="s">
         <v>17</v>
       </c>
@@ -2182,7 +2182,7 @@
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="1" t="s">
         <v>18</v>
       </c>
@@ -2227,7 +2227,7 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2274,7 +2274,7 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A38" s="8"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="1" t="s">
         <v>17</v>
       </c>
@@ -2294,16 +2294,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A38"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A37:A38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2365,7 +2365,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2406,7 +2406,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2445,7 +2445,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
@@ -2484,7 +2484,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
@@ -2523,7 +2523,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2564,7 +2564,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
@@ -2603,7 +2603,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
@@ -2642,7 +2642,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
@@ -2681,7 +2681,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2722,7 +2722,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
@@ -2761,7 +2761,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
@@ -2800,7 +2800,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
@@ -2839,7 +2839,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2880,7 +2880,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
@@ -2919,7 +2919,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
@@ -2958,7 +2958,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2997,7 +2997,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -3038,7 +3038,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
@@ -3077,7 +3077,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
@@ -3116,7 +3116,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
@@ -3155,7 +3155,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -3196,7 +3196,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
@@ -3235,7 +3235,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
@@ -3274,7 +3274,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="1" t="s">
         <v>18</v>
       </c>
@@ -3313,7 +3313,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -3354,7 +3354,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="1" t="s">
         <v>16</v>
       </c>
@@ -3393,7 +3393,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="1" t="s">
         <v>17</v>
       </c>
@@ -3432,7 +3432,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="1" t="s">
         <v>18</v>
       </c>
@@ -3471,7 +3471,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -3512,7 +3512,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="1" t="s">
         <v>16</v>
       </c>
@@ -3551,7 +3551,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
@@ -3590,7 +3590,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="1" t="s">
         <v>18</v>
       </c>

</xml_diff>